<commit_message>
Upgrade to POI 3.8 - Final
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/DateFormatTests.xlsx
+++ b/test-data/spreadsheet/DateFormatTests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="33140" windowHeight="22740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20610" windowHeight="11640" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Flags" sheetId="2" r:id="rId1"/>
     <sheet name="Tests" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -181,26 +181,18 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Debug</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>False</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>h:m</t>
+  </si>
+  <si>
+    <t>True</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="dd\-mmm\-yyyy\ hh:mm:ss.000"/>
-    <numFmt numFmtId="170" formatCode="@"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy\ hh:mm:ss.000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -276,13 +268,13 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -616,20 +608,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="7"/>
+    <col min="1" max="1" width="10.75" style="7"/>
     <col min="2" max="2" width="17" style="8" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="10.7109375" style="1"/>
+    <col min="3" max="3" width="34.875" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="10.75" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1">
@@ -655,14 +647,12 @@
       <c r="A3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="B3" s="7"/>
       <c r="C3" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="25.5">
       <c r="A4" s="7" t="s">
         <v>37</v>
       </c>
@@ -686,22 +676,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.75" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="10.7109375" style="2"/>
+    <col min="5" max="16384" width="10.75" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1">
@@ -1319,13 +1309,19 @@
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="9" t="str">
+      <c r="A42" s="11" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="7"/>
+        <v>14:35</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="10">
+        <v>17816.607951388887</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
zk-poi upgrade to PIO 3.8-Final(merge)
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/DateFormatTests.xlsx
+++ b/test-data/spreadsheet/DateFormatTests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="33140" windowHeight="22740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20610" windowHeight="11640" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Flags" sheetId="2" r:id="rId1"/>
     <sheet name="Tests" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -181,26 +181,18 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Debug</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>False</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>h:m</t>
+  </si>
+  <si>
+    <t>True</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="dd\-mmm\-yyyy\ hh:mm:ss.000"/>
-    <numFmt numFmtId="170" formatCode="@"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy\ hh:mm:ss.000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -276,13 +268,13 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -616,20 +608,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="7"/>
+    <col min="1" max="1" width="10.75" style="7"/>
     <col min="2" max="2" width="17" style="8" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="10.7109375" style="1"/>
+    <col min="3" max="3" width="34.875" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="10.75" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1">
@@ -655,14 +647,12 @@
       <c r="A3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="B3" s="7"/>
       <c r="C3" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="25.5">
       <c r="A4" s="7" t="s">
         <v>37</v>
       </c>
@@ -686,22 +676,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.75" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="10.7109375" style="2"/>
+    <col min="5" max="16384" width="10.75" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1">
@@ -1319,13 +1309,19 @@
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="9" t="str">
+      <c r="A42" s="11" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="7"/>
+        <v>14:35</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="10">
+        <v>17816.607951388887</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>